<commit_message>
update template & testing for 941x
</commit_message>
<xml_diff>
--- a/941X_data_template.xlsx
+++ b/941X_data_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -46,7 +46,10 @@
     <t xml:space="preserve">Sign Name, Title, Phone</t>
   </si>
   <si>
-    <t xml:space="preserve">Corrected</t>
+    <t xml:space="preserve">Total_Wages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qualified_Wages</t>
   </si>
   <si>
     <t xml:space="preserve">09-09-2022</t>
@@ -230,13 +233,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="15.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.99"/>
@@ -244,6 +247,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -275,10 +279,13 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2020</v>
@@ -287,27 +294,30 @@
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>1231.22</v>
       </c>
+      <c r="J2" s="0" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2021</v>
@@ -316,22 +326,25 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>123</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>10231.23</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>8000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>